<commit_message>
Updating Team Test Cases
</commit_message>
<xml_diff>
--- a/TestData/RebootTest.xlsx
+++ b/TestData/RebootTest.xlsx
@@ -9,6 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Reboot" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="City" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
   <si>
     <t xml:space="preserve">BuildingProjectID</t>
   </si>
@@ -67,7 +68,10 @@
     <t xml:space="preserve">RecertificationBuildingProject</t>
   </si>
   <si>
-    <t xml:space="preserve">100019359</t>
+    <t xml:space="preserve">TeamMember</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1000193599</t>
   </si>
   <si>
     <t xml:space="preserve">1000193627</t>
@@ -92,6 +96,63 @@
   </si>
   <si>
     <t xml:space="preserve">1000193632</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qashree15@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CityProjectName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CityGrossAreaMiles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CityPopulation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CityAddress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">City_City</t>
+  </si>
+  <si>
+    <t xml:space="preserve">City_Country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">City_State</t>
+  </si>
+  <si>
+    <t xml:space="preserve">City_Zipcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CityProjectId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TestCity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19305</t>
+  </si>
+  <si>
+    <t xml:space="preserve">45000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2101 L St NW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Washington</t>
+  </si>
+  <si>
+    <t xml:space="preserve">United States</t>
+  </si>
+  <si>
+    <t xml:space="preserve">District of Columbia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20037</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8000004308</t>
   </si>
 </sst>
 </file>
@@ -125,8 +186,10 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -171,8 +234,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -197,13 +264,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O2" activeCellId="0" sqref="O2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.64"/>
@@ -215,6 +282,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="19.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="18.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="25.19"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -263,55 +331,64 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="P1" s="0" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C2" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>16</v>
-      </c>
       <c r="G2" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="O2" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="N2" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="O2" s="0" t="s">
-        <v>17</v>
+      <c r="P2" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="P2" r:id="rId1" display="qashree15@gmail.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -320,4 +397,91 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.56"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
changes test cases description
</commit_message>
<xml_diff>
--- a/TestData/RebootTest.xlsx
+++ b/TestData/RebootTest.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Reboot" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="48">
   <si>
     <t xml:space="preserve">BuildingProjectID</t>
   </si>
@@ -128,13 +128,19 @@
     <t xml:space="preserve">CityProjectId</t>
   </si>
   <si>
+    <t xml:space="preserve">UpdatedByEmailId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TONS/YEAR/CAPITA</t>
+  </si>
+  <si>
     <t xml:space="preserve">TestCity</t>
   </si>
   <si>
-    <t xml:space="preserve">19305</t>
-  </si>
-  <si>
-    <t xml:space="preserve">45000</t>
+    <t xml:space="preserve">1000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5000</t>
   </si>
   <si>
     <t xml:space="preserve">2101 L St NW</t>
@@ -153,6 +159,12 @@
   </si>
   <si>
     <t xml:space="preserve">8000004308</t>
+  </si>
+  <si>
+    <t xml:space="preserve">narayanarc21@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15</t>
   </si>
 </sst>
 </file>
@@ -266,11 +278,11 @@
   </sheetPr>
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.64"/>
@@ -404,17 +416,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="22.79"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -445,37 +458,52 @@
       <c r="I1" s="0" t="s">
         <v>34</v>
       </c>
+      <c r="J1" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J2" r:id="rId1" display="narayanarc21@gmail.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Test data file updated
</commit_message>
<xml_diff>
--- a/TestData/RebootTest.xlsx
+++ b/TestData/RebootTest.xlsx
@@ -5,12 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Reboot" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="ProjectRegistration" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="City" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Communities" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="City1" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="107">
   <si>
     <t xml:space="preserve">BuildingProjectID</t>
   </si>
@@ -78,7 +80,7 @@
     <t xml:space="preserve">1000193627</t>
   </si>
   <si>
-    <t xml:space="preserve">8000004236</t>
+    <t xml:space="preserve">1000194044</t>
   </si>
   <si>
     <t xml:space="preserve">8000004271</t>
@@ -126,6 +128,9 @@
     <t xml:space="preserve">City_Zipcode</t>
   </si>
   <si>
+    <t xml:space="preserve">CommunitiesProjectName</t>
+  </si>
+  <si>
     <t xml:space="preserve">TestCity</t>
   </si>
   <si>
@@ -150,12 +155,183 @@
     <t xml:space="preserve">20037</t>
   </si>
   <si>
+    <t xml:space="preserve">TestCommunities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UpdatedByEmailId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Population_Comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ProjectArea_Comments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EnergyTONS_YEAR_CAPITA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy_Comments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water_Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WaterUnit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water_Duration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water_Comments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Waste_Generation_TONS_YEAR_CAPITA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Waste_Gen_Comments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Waste_Diversion_Percent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Waste_Div_Comments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transport_Miles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transport_Comments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HealthAndSafety_Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HealthAndSafety_Remarks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edutcation_Bachelor_Population_Percent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edutcation_Bachelor_Population_Remarks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Equitability_Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Equitability_Remarks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edutcation_HighSchool_Population_Percent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edutcation_HighSchool_Population_Remarks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ProsperityMedianIncome_USDollar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ProsperityMedianIncome_USDollar_Remarks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Equitability_MedianGrossIncome_Percent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Equitability_MedianGrossIncome_Remarks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ProsperityUnemploymentRate_Percent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ProsperityUnemploymentRate_Remarks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HealthSafetySensitiveGrp_value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HealthSafetySensitiveGrp_value _Remarks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HealthSafetyVoilentCrime_value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HealthSafetyVoilentCrime _Remarks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">narayanarc21@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Init@pass1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Population Remarks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project Area Remarks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy Remarks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gallons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Per Year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water Consumption Remarks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Waste Generation Remarks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Waste Diversion Remarks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transportation Remarks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">150</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">900</t>
+  </si>
+  <si>
+    <t xml:space="preserve">60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">400</t>
+  </si>
+  <si>
     <t xml:space="preserve">CityProjectId</t>
   </si>
   <si>
-    <t xml:space="preserve">UpdatedByEmailId</t>
-  </si>
-  <si>
     <t xml:space="preserve">TONS_YEAR_CAPITA </t>
   </si>
   <si>
@@ -165,163 +341,10 @@
     <t xml:space="preserve">NextYear_TONS_YEAR_CAPITA</t>
   </si>
   <si>
-    <t xml:space="preserve">Water_Value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WaterUnit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Water_Duration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Population_Comment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ProjectArea_Comments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Waste_Generation_TONS_YEAR_CAPITA </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Waste_Diversion_Percent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Energy_Comments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Water_Comments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Waste_Gen_Comments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Waste_Div_Comments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transport_Miles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transport_Comments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HealthAndSafety_Value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HealthAndSafety_Remarks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Edutcation_Bachelor_Population_Percent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Equitability_Value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Equitability_Remarks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Edutcation_Bachelor_Population_Remarks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ProsperityMedianIncome_USDollar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ProsperityMedianIncome_USDollar_Remarks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Equitability_MedianGrossIncome_Percent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Equitability_MedianGrossIncome_Remarks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ProsperityUnemploymentRate_Percent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ProsperityUnemploymentRate_Remarks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HealthSafetySensitiveGrp_value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HealthSafetySensitiveGrp_value _Remarks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HealthSafetyVoilentCrime_value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HealthSafetyVoilentCrime _Remarks</t>
-  </si>
-  <si>
     <t xml:space="preserve">8000004308</t>
   </si>
   <si>
-    <t xml:space="preserve">narayanarc21@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10</t>
-  </si>
-  <si>
     <t xml:space="preserve">11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gallons</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Per Year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Population Remarks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Project Area Remarks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Energy Remarks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Water Consumption Remarks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Waste Generation Remarks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Waste Diversion Remarks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transportation Remarks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">150</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">70</t>
-  </si>
-  <si>
-    <t xml:space="preserve">900</t>
-  </si>
-  <si>
-    <t xml:space="preserve">60</t>
-  </si>
-  <si>
-    <t xml:space="preserve">400</t>
   </si>
 </sst>
 </file>
@@ -331,7 +354,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -359,6 +382,13 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FF2A00FF"/>
+      <name val="Consolas"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -403,7 +433,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -416,6 +446,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,6 +459,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF2A00FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -435,11 +529,11 @@
   </sheetPr>
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.64"/>
@@ -573,13 +667,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -606,31 +700,42 @@
       <c r="H1" s="0" t="s">
         <v>33</v>
       </c>
+      <c r="I1" s="0" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I3" s="0" t="n">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -649,13 +754,583 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:AH3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="20.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="27.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="23.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="21.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="24.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="18.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1016" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q1" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="R1" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="T1" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="U1" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="V1" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="W1" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="X1" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y1" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z1" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA1" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC1" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE1" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AG1" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q2" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="R2" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="S2" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="T2" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="U2" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="V2" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="W2" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="X2" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y2" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="Z2" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA2" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC2" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE2" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AG2" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I3" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="M3" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="O3" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="Q3" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="S3" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="U3" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="W3" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="Y3" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="AA3" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="AC3" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="AE3" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="narayanarc21@gmail.com"/>
+    <hyperlink ref="B2" r:id="rId2" display="Init@pass1"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AH3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="20.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="27.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="23.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="21.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="24.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="18.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1016" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q1" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="R1" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="T1" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="U1" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="V1" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="W1" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="X1" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y1" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z1" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA1" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC1" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE1" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AG1" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q2" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="R2" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="S2" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="T2" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="U2" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="V2" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="W2" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="X2" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y2" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="Z2" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA2" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC2" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE2" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AG2" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I3" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="M3" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="O3" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="Q3" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="S3" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="U3" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="W3" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="Y3" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="AA3" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="AC3" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="AE3" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="narayanarc21@gmail.com"/>
+    <hyperlink ref="B2" r:id="rId2" display="Init@pass1"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:AQ2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.67"/>
@@ -692,49 +1367,49 @@
         <v>33</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>42</v>
+        <v>101</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>44</v>
+        <v>102</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>45</v>
+        <v>103</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q1" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="R1" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="O1" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="P1" s="0" t="s">
+      <c r="S1" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="T1" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="U1" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="Q1" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="R1" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="S1" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="T1" s="0" t="s">
+      <c r="V1" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="U1" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="V1" s="0" t="s">
+      <c r="W1" s="0" t="s">
         <v>55</v>
-      </c>
-      <c r="W1" s="0" t="s">
-        <v>56</v>
       </c>
       <c r="X1" s="0" t="s">
         <v>57</v>
@@ -755,177 +1430,177 @@
         <v>62</v>
       </c>
       <c r="AD1" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AE1" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AF1" s="0" t="s">
         <v>62</v>
       </c>
       <c r="AG1" s="0" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="AH1" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="AI1" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="AJ1" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="AL1" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="AN1" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="AP1" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="M2" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q2" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="N2" s="0" t="s">
+      <c r="R2" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="O2" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="P2" s="0" t="s">
+      <c r="S2" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="T2" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="U2" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="Q2" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="R2" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="S2" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="T2" s="0" t="s">
+      <c r="V2" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="U2" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="V2" s="0" t="s">
+      <c r="W2" s="0" t="s">
         <v>89</v>
-      </c>
-      <c r="W2" s="0" t="s">
-        <v>90</v>
       </c>
       <c r="X2" s="0" t="s">
         <v>91</v>
       </c>
       <c r="Y2" s="0" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="Z2" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AA2" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AB2" s="0" t="s">
         <v>61</v>
       </c>
       <c r="AC2" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="AD2" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AE2" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AF2" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AG2" s="0" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="AH2" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="AI2" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="AJ2" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AK2" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="AL2" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AM2" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="AN2" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AO2" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="AP2" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AQ2" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated Reboot sml and xlsx
</commit_message>
<xml_diff>
--- a/TestData/RebootTest.xlsx
+++ b/TestData/RebootTest.xlsx
@@ -512,7 +512,7 @@
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
+      <selection pane="topLeft" activeCell="O2" activeCellId="0" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -624,7 +624,7 @@
         <v>24</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="P2" s="2" t="s">
         <v>25</v>
@@ -652,7 +652,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
+      <selection pane="topLeft" activeCell="I3" activeCellId="1" sqref="O2 I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -739,7 +739,7 @@
   <dimension ref="A1:AH3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="1" sqref="O2 C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1024,7 +1024,7 @@
   <dimension ref="A1:AH3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="O2 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Changing Extentreport Testdata smlsuite
</commit_message>
<xml_diff>
--- a/TestData/RebootTest.xlsx
+++ b/TestData/RebootTest.xlsx
@@ -511,7 +511,7 @@
   </sheetPr>
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="O2" activeCellId="0" sqref="O2"/>
     </sheetView>
   </sheetViews>
@@ -624,7 +624,7 @@
         <v>24</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="P2" s="2" t="s">
         <v>25</v>

</xml_diff>